<commit_message>
TMTT0042714_VerificationOfBuyersListFeatureOnEngagementScreen - 21 April - Final
</commit_message>
<xml_diff>
--- a/TestData/TMTT0042714_VerificationOfBuyersListFeatureOnEngagementScreen.xlsx
+++ b/TestData/TMTT0042714_VerificationOfBuyersListFeatureOnEngagementScreen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176B8D4D-6A1F-4383-A03C-7B6526129881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C83711C-D4FE-42C4-BC51-85F75AEE9ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" tabRatio="468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
   <si>
     <t>Subject</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>StandardTestCompany</t>
+  </si>
+  <si>
+    <t>CaoUser</t>
+  </si>
+  <si>
+    <t>Gemma Hardy</t>
   </si>
 </sst>
 </file>
@@ -613,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,20 +631,26 @@
     <col min="2" max="2" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -964,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01CAA37-8A09-4C20-87A8-FA8EE6CE15FC}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>